<commit_message>
use linked list to store mail ids
</commit_message>
<xml_diff>
--- a/prefix_analysis.xlsx
+++ b/prefix_analysis.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud_Drive\Codes\Github_Repos\DSA_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{3134A1AD-102E-4098-AF11-510A1CA6BCFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31ECBC0-37BB-4FB8-AD62-6BB59E68B9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="22932" yWindow="-1968" windowWidth="14616" windowHeight="22656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prefix_result" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -127,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -295,7 +306,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -473,6 +484,42 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -720,17 +767,32 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="49" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="37" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -5165,6 +5227,11 @@
       <a:endParaRPr lang="zh-TW"/>
     </a:p>
   </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
@@ -12062,11 +12129,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N33" sqref="N33"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12097,11 +12164,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3">
-        <f>C2/$C$39</f>
+      <c r="B2" s="2">
+        <f t="shared" ref="B2:B37" si="0">C2/$C$39</f>
         <v>0.13680119762829629</v>
       </c>
       <c r="C2" s="1">
@@ -12111,707 +12178,707 @@
         <f>LOG(B2)</f>
         <v>-0.86391010056119699</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <f>SUM(B2:$B$37)</f>
         <v>1.0000000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3">
-        <f>C3/$C$39</f>
+      <c r="B3" s="2">
+        <f t="shared" si="0"/>
         <v>0.11258633825862134</v>
       </c>
       <c r="C3" s="1">
         <v>378588</v>
       </c>
       <c r="D3" s="1">
-        <f t="shared" ref="D3:D37" si="0">LOG(B3)</f>
+        <f t="shared" ref="D3:D37" si="1">LOG(B3)</f>
         <v>-0.94851430556692251</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <f>SUM(B3:$B$37)</f>
         <v>0.86319880237170388</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="3">
-        <f>C4/$C$39</f>
+      <c r="B4" s="2">
+        <f t="shared" si="0"/>
         <v>6.8413683747858084E-2</v>
       </c>
       <c r="C4" s="1">
         <v>230051</v>
       </c>
       <c r="D4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.164857024276589</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <f>SUM(B4:$B$37)</f>
         <v>0.75061246411308258</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3">
-        <f>C5/$C$39</f>
+      <c r="B5" s="2">
+        <f t="shared" si="0"/>
         <v>6.795511629829605E-2</v>
       </c>
       <c r="C5" s="1">
         <v>228509</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.167777839940024</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <f>SUM(B5:$B$37)</f>
         <v>0.68219878036522441</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="3">
-        <f>C6/$C$39</f>
+      <c r="B6" s="2">
+        <f t="shared" si="0"/>
         <v>6.6476816173929698E-2</v>
       </c>
       <c r="C6" s="1">
         <v>223538</v>
       </c>
       <c r="D6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.1773297887306382</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6" s="2">
         <f>SUM(B6:$B$37)</f>
         <v>0.61424366406692832</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="3">
-        <f>C7/$C$39</f>
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
         <v>5.1797899630231667E-2</v>
       </c>
       <c r="C7" s="1">
         <v>174178</v>
       </c>
       <c r="D7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.2856878502450029</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <f>SUM(B7:$B$37)</f>
         <v>0.54776684789299857</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="3">
-        <f>C8/$C$39</f>
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
         <v>5.1695599239408488E-2</v>
       </c>
       <c r="C8" s="1">
         <v>173834</v>
       </c>
       <c r="D8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.2865464261011932</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <f>SUM(B8:$B$37)</f>
         <v>0.49596894826276688</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="3">
-        <f>C9/$C$39</f>
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
         <v>4.2660452512693875E-2</v>
       </c>
       <c r="C9" s="1">
         <v>143452</v>
       </c>
       <c r="D9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3699745421654546</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <f>SUM(B9:$B$37)</f>
         <v>0.44427334902335841</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3">
-        <f>C10/$C$39</f>
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
         <v>4.1951189628643637E-2</v>
       </c>
       <c r="C10" s="1">
         <v>141067</v>
       </c>
       <c r="D10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3772557191778327</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <f>SUM(B10:$B$37)</f>
         <v>0.40161289651066451</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="3">
-        <f>C11/$C$39</f>
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
         <v>4.147240000880259E-2</v>
       </c>
       <c r="C11" s="1">
         <v>139457</v>
       </c>
       <c r="D11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.382240831276454</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <f>SUM(B11:$B$37)</f>
         <v>0.35966170688202087</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3">
-        <f>C12/$C$39</f>
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
         <v>4.0571918661672979E-2</v>
       </c>
       <c r="C12" s="1">
         <v>136429</v>
       </c>
       <c r="D12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.3917744538565757</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <f>SUM(B12:$B$37)</f>
         <v>0.31818930687321828</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
-        <f>C13/$C$39</f>
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
         <v>3.5446490650517477E-2</v>
       </c>
       <c r="C13" s="1">
         <v>119194</v>
       </c>
       <c r="D13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.4504267553062604</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <f>SUM(B13:$B$37)</f>
         <v>0.27761738821154525</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="3">
-        <f>C14/$C$39</f>
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
         <v>3.3021614526179681E-2</v>
       </c>
       <c r="C14" s="1">
         <v>111040</v>
       </c>
       <c r="D14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.481201696589002</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <f>SUM(B14:$B$37)</f>
         <v>0.2421708975610278</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B15" s="3">
-        <f>C15/$C$39</f>
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
         <v>2.8414230935995047E-2</v>
       </c>
       <c r="C15" s="1">
         <v>95547</v>
       </c>
       <c r="D15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.5464640941423404</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <f>SUM(B15:$B$37)</f>
         <v>0.20914928303484814</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="3">
-        <f>C16/$C$39</f>
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
         <v>2.393561498891052E-2</v>
       </c>
       <c r="C16" s="1">
         <v>80487</v>
       </c>
       <c r="D16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.6209554095081635</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <f>SUM(B16:$B$37)</f>
         <v>0.1807350520988531</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="5">
         <v>1</v>
       </c>
-      <c r="B17" s="3">
-        <f>C17/$C$39</f>
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
         <v>2.23267629123018E-2</v>
       </c>
       <c r="C17" s="1">
         <v>75077</v>
       </c>
       <c r="D17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.6511742393663003</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <f>SUM(B17:$B$37)</f>
         <v>0.15679943710994257</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="3">
-        <f>C18/$C$39</f>
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
         <v>2.2190263262918546E-2</v>
       </c>
       <c r="C18" s="1">
         <v>74618</v>
       </c>
       <c r="D18" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.6538375453139769</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <f>SUM(B18:$B$37)</f>
         <v>0.13447267419764078</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="3">
-        <f>C19/$C$39</f>
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
         <v>1.9771632220578674E-2</v>
       </c>
       <c r="C19" s="1">
         <v>66485</v>
       </c>
       <c r="D19" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.7039574766079217</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <f>SUM(B19:$B$37)</f>
         <v>0.11228241093472223</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="3">
-        <f>C20/$C$39</f>
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
         <v>1.6692509410743801E-2</v>
       </c>
       <c r="C20" s="1">
         <v>56131</v>
       </c>
       <c r="D20" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.7774783702520085</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <f>SUM(B20:$B$37)</f>
         <v>9.2510778714143579E-2</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
-        <f>C21/$C$39</f>
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
         <v>1.2135383861399625E-2</v>
       </c>
       <c r="C21" s="1">
         <v>40807</v>
       </c>
       <c r="D21" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.9159464816929026</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E21" s="2">
         <f>SUM(B21:$B$37)</f>
         <v>7.5818269303399771E-2</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="4">
         <v>2</v>
       </c>
-      <c r="B22" s="3">
-        <f>C22/$C$39</f>
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
         <v>1.2095831675412755E-2</v>
       </c>
       <c r="C22" s="1">
         <v>40674</v>
       </c>
       <c r="D22" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-1.9173642654066956</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E22" s="2">
         <f>SUM(B22:$B$37)</f>
         <v>6.3682885442000153E-2</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="3">
-        <f>C23/$C$39</f>
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
         <v>8.2539167072597005E-3</v>
       </c>
       <c r="C23" s="1">
         <v>27755</v>
       </c>
       <c r="D23" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.0833399180319021</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E23" s="2">
         <f>SUM(B23:$B$37)</f>
         <v>5.1587053766587398E-2</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="3">
-        <f>C24/$C$39</f>
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
         <v>7.6805587028786256E-3</v>
       </c>
       <c r="C24" s="1">
         <v>25827</v>
       </c>
       <c r="D24" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.1146071871622611</v>
       </c>
-      <c r="E24" s="3">
+      <c r="E24" s="2">
         <f>SUM(B24:$B$37)</f>
         <v>4.3333137059327696E-2</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="3">
-        <f>C25/$C$39</f>
+      <c r="B25" s="2">
+        <f t="shared" si="0"/>
         <v>7.260651284732321E-3</v>
       </c>
       <c r="C25" s="1">
         <v>24415</v>
       </c>
       <c r="D25" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.1390244210796396</v>
       </c>
-      <c r="E25" s="3">
+      <c r="E25" s="2">
         <f>SUM(B25:$B$37)</f>
         <v>3.5652578356449062E-2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="3">
-        <f>C26/$C$39</f>
+      <c r="B26" s="2">
+        <f t="shared" si="0"/>
         <v>4.6029228173289725E-3</v>
       </c>
       <c r="C26" s="1">
         <v>15478</v>
       </c>
       <c r="D26" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.3369663073761018</v>
       </c>
-      <c r="E26" s="3">
+      <c r="E26" s="2">
         <f>SUM(B26:$B$37)</f>
         <v>2.8391927071716734E-2</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
+      <c r="A27" s="3">
         <v>3</v>
       </c>
-      <c r="B27" s="3">
-        <f>C27/$C$39</f>
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
         <v>4.4812924107979256E-3</v>
       </c>
       <c r="C27" s="1">
         <v>15069</v>
       </c>
       <c r="D27" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.3485967168205701</v>
       </c>
-      <c r="E27" s="3">
+      <c r="E27" s="2">
         <f>SUM(B27:$B$37)</f>
         <v>2.3789004254387763E-2</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="A28" s="3">
         <v>4</v>
       </c>
-      <c r="B28" s="3">
-        <f>C28/$C$39</f>
+      <c r="B28" s="2">
+        <f t="shared" si="0"/>
         <v>3.6025201582325348E-3</v>
       </c>
       <c r="C28" s="1">
         <v>12114</v>
       </c>
       <c r="D28" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.4433935803724989</v>
       </c>
-      <c r="E28" s="3">
+      <c r="E28" s="2">
         <f>SUM(B28:$B$37)</f>
         <v>1.9307711843589839E-2</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="A29" s="3">
         <v>5</v>
       </c>
-      <c r="B29" s="3">
-        <f>C29/$C$39</f>
+      <c r="B29" s="2">
+        <f t="shared" si="0"/>
         <v>3.112132528966772E-3</v>
       </c>
       <c r="C29" s="1">
         <v>10465</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.5069419170250766</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E29" s="2">
         <f>SUM(B29:$B$37)</f>
         <v>1.5705191685357302E-2</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="3">
         <v>6</v>
       </c>
-      <c r="B30" s="3">
-        <f>C30/$C$39</f>
+      <c r="B30" s="2">
+        <f t="shared" si="0"/>
         <v>2.5060621903108446E-3</v>
       </c>
       <c r="C30" s="1">
         <v>8427</v>
       </c>
       <c r="D30" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.6010081557785414</v>
       </c>
-      <c r="E30" s="3">
+      <c r="E30" s="2">
         <f>SUM(B30:$B$37)</f>
         <v>1.2593059156390533E-2</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="3">
         <v>7</v>
       </c>
-      <c r="B31" s="3">
-        <f>C31/$C$39</f>
+      <c r="B31" s="2">
+        <f t="shared" si="0"/>
         <v>2.0840730781652305E-3</v>
       </c>
       <c r="C31" s="1">
         <v>7008</v>
       </c>
       <c r="D31" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.6810870565397575</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E31" s="2">
         <f>SUM(B31:$B$37)</f>
         <v>1.0086996966079688E-2</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="A32" s="3">
         <v>8</v>
       </c>
-      <c r="B32" s="3">
-        <f>C32/$C$39</f>
+      <c r="B32" s="2">
+        <f t="shared" si="0"/>
         <v>1.7923385334049436E-3</v>
       </c>
       <c r="C32" s="1">
         <v>6027</v>
       </c>
       <c r="D32" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.74657995823187</v>
       </c>
-      <c r="E32" s="3">
+      <c r="E32" s="2">
         <f>SUM(B32:$B$37)</f>
         <v>8.0029238879144576E-3</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="A33" s="3">
         <v>0</v>
       </c>
-      <c r="B33" s="3">
-        <f>C33/$C$39</f>
+      <c r="B33" s="2">
+        <f t="shared" si="0"/>
         <v>1.695985839722647E-3</v>
       </c>
       <c r="C33" s="1">
         <v>5703</v>
       </c>
       <c r="D33" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.7705777781146761</v>
       </c>
-      <c r="E33" s="3">
+      <c r="E33" s="2">
         <f>SUM(B33:$B$37)</f>
         <v>6.210585354509514E-3</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="3">
         <v>9</v>
       </c>
-      <c r="B34" s="3">
-        <f>C34/$C$39</f>
+      <c r="B34" s="2">
+        <f t="shared" si="0"/>
         <v>1.6347245591715571E-3</v>
       </c>
       <c r="C34" s="1">
         <v>5497</v>
       </c>
       <c r="D34" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.7865554127340513</v>
       </c>
-      <c r="E34" s="3">
+      <c r="E34" s="2">
         <f>SUM(B34:$B$37)</f>
         <v>4.514599514786867E-3</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B35" s="3">
-        <f>C35/$C$39</f>
+      <c r="B35" s="2">
+        <f t="shared" si="0"/>
         <v>1.4726498120825088E-3</v>
       </c>
       <c r="C35" s="1">
         <v>4952</v>
       </c>
       <c r="D35" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-2.83190051368772</v>
       </c>
-      <c r="E35" s="3">
+      <c r="E35" s="2">
         <f>SUM(B35:$B$37)</f>
         <v>2.8798749556153101E-3</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B36" s="3">
-        <f>C36/$C$39</f>
+      <c r="B36" s="2">
+        <f t="shared" si="0"/>
         <v>9.2754336912062704E-4</v>
       </c>
       <c r="C36" s="1">
         <v>3119</v>
       </c>
       <c r="D36" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.0326657749426378</v>
       </c>
-      <c r="E36" s="3">
+      <c r="E36" s="2">
         <f>SUM(B36:$B$37)</f>
         <v>1.4072251435328013E-3</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="3">
-        <f>C37/$C$39</f>
+      <c r="B37" s="2">
+        <f t="shared" si="0"/>
         <v>4.7968177441217423E-4</v>
       </c>
       <c r="C37" s="1">
         <v>1613</v>
       </c>
       <c r="D37" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>-3.3190467823108203</v>
       </c>
-      <c r="E37" s="3">
+      <c r="E37" s="2">
         <f>SUM(B37:$B$37)</f>
         <v>4.7968177441217423E-4</v>
       </c>

</xml_diff>

<commit_message>
handle adding one mail multiple times
</commit_message>
<xml_diff>
--- a/prefix_analysis.xlsx
+++ b/prefix_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud_Drive\Codes\Github_Repos\DSA_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31ECBC0-37BB-4FB8-AD62-6BB59E68B9CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94068165-74B0-4A37-AD81-AB1C9183AE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-1968" windowWidth="14616" windowHeight="22656" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="prefix_result" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>a</t>
   </si>
@@ -119,19 +119,15 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>sum</t>
-    <phoneticPr fontId="18" type="noConversion"/>
-  </si>
-  <si>
     <t>ratio</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>log</t>
+    <t>accumilate ratio</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>accumilate ratio</t>
+    <t>accumilate count</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -5242,506 +5238,6 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="zh-TW" altLang="en-US">
-                <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-                <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-              </a:rPr>
-              <a:t>字首出現頻率</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-TW">
-                <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-                <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-              </a:rPr>
-              <a:t>(</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="zh-TW" altLang="en-US">
-                <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-                <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-              </a:rPr>
-              <a:t>對數</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" altLang="zh-TW">
-                <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-                <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-              </a:rPr>
-              <a:t>)</a:t>
-            </a:r>
-            <a:endParaRPr lang="zh-TW" altLang="en-US">
-              <a:latin typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-              <a:ea typeface="微軟正黑體" panose="020B0604030504040204" pitchFamily="34" charset="-120"/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="zh-TW"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>prefix_result!$A$2:$A$37</c:f>
-              <c:strCache>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>t</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>a</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>s</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>o</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>i</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>c</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>w</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>b</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>p</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>f</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>h</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>m</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>r</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>d</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>l</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>e</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>n</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>g</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>u</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>v</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>j</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>k</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>y</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>7</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>9</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>q</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>z</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>x</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>prefix_result!$D$2:$D$37</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="36"/>
-                <c:pt idx="0">
-                  <c:v>-0.86391010056119699</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>-0.94851430556692251</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>-1.164857024276589</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>-1.167777839940024</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>-1.1773297887306382</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>-1.2856878502450029</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>-1.2865464261011932</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>-1.3699745421654546</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>-1.3772557191778327</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>-1.382240831276454</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>-1.3917744538565757</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>-1.4504267553062604</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>-1.481201696589002</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>-1.5464640941423404</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>-1.6209554095081635</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>-1.6511742393663003</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>-1.6538375453139769</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>-1.7039574766079217</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>-1.7774783702520085</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>-1.9159464816929026</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>-1.9173642654066956</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>-2.0833399180319021</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>-2.1146071871622611</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>-2.1390244210796396</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>-2.3369663073761018</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>-2.3485967168205701</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>-2.4433935803724989</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>-2.5069419170250766</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>-2.6010081557785414</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>-2.6810870565397575</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>-2.74657995823187</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>-2.7705777781146761</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>-2.7865554127340513</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>-2.83190051368772</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>-3.0326657749426378</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>-3.3190467823108203</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3CA8-4C98-B60C-D835170301BF}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:smooth val="0"/>
-        <c:axId val="2118322832"/>
-        <c:axId val="2118323248"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="2118322832"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="1"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118323248"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2118323248"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="-0.5"/>
-          <c:min val="-3.5"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="zh-TW"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2118322832"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="zh-TW"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="zh-TW"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
       <c14:style val="108"/>
     </mc:Choice>
     <mc:Fallback>
@@ -5939,7 +5435,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$2</c:f>
+              <c:f>prefix_result!$D$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -6059,7 +5555,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$3</c:f>
+              <c:f>prefix_result!$D$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -6179,7 +5675,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$4</c:f>
+              <c:f>prefix_result!$D$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -6299,7 +5795,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$5</c:f>
+              <c:f>prefix_result!$D$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -6419,7 +5915,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$6</c:f>
+              <c:f>prefix_result!$D$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -6539,7 +6035,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$7</c:f>
+              <c:f>prefix_result!$D$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -6659,7 +6155,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$8</c:f>
+              <c:f>prefix_result!$D$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -6779,7 +6275,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$9</c:f>
+              <c:f>prefix_result!$D$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -6899,7 +6395,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$10</c:f>
+              <c:f>prefix_result!$D$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7019,7 +6515,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$11</c:f>
+              <c:f>prefix_result!$D$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7139,7 +6635,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$12</c:f>
+              <c:f>prefix_result!$D$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7259,7 +6755,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$13</c:f>
+              <c:f>prefix_result!$D$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7379,7 +6875,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$14</c:f>
+              <c:f>prefix_result!$D$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7499,7 +6995,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$15</c:f>
+              <c:f>prefix_result!$D$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7619,7 +7115,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$16</c:f>
+              <c:f>prefix_result!$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7739,7 +7235,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$17</c:f>
+              <c:f>prefix_result!$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7859,7 +7355,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$18</c:f>
+              <c:f>prefix_result!$D$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -7979,7 +7475,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$19</c:f>
+              <c:f>prefix_result!$D$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -8099,7 +7595,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$20</c:f>
+              <c:f>prefix_result!$D$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -8219,7 +7715,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$21</c:f>
+              <c:f>prefix_result!$D$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -8339,7 +7835,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$22</c:f>
+              <c:f>prefix_result!$D$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -8459,7 +7955,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$23</c:f>
+              <c:f>prefix_result!$D$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -8579,7 +8075,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$24</c:f>
+              <c:f>prefix_result!$D$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -8699,7 +8195,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$25</c:f>
+              <c:f>prefix_result!$D$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -8819,7 +8315,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$26</c:f>
+              <c:f>prefix_result!$D$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -8939,7 +8435,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$27</c:f>
+              <c:f>prefix_result!$D$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9043,7 +8539,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$28</c:f>
+              <c:f>prefix_result!$D$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9147,7 +8643,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$29</c:f>
+              <c:f>prefix_result!$D$29</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9251,7 +8747,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$30</c:f>
+              <c:f>prefix_result!$D$30</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9355,7 +8851,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$31</c:f>
+              <c:f>prefix_result!$D$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9459,7 +8955,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$32</c:f>
+              <c:f>prefix_result!$D$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9563,7 +9059,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$33</c:f>
+              <c:f>prefix_result!$D$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9667,7 +9163,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$34</c:f>
+              <c:f>prefix_result!$D$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9771,7 +9267,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$35</c:f>
+              <c:f>prefix_result!$D$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9875,7 +9371,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$36</c:f>
+              <c:f>prefix_result!$D$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -9979,7 +9475,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$E$37</c:f>
+              <c:f>prefix_result!$D$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
@@ -10141,46 +9637,6 @@
 </file>
 
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
   <a:schemeClr val="accent6"/>
 </cs:colorStyle>
@@ -10695,522 +10151,6 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -11722,16 +10662,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11758,52 +10698,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>190499</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="圖表 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CBA5C60F-BEAE-4E2F-BD67-C5818DE79AA9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>247649</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11824,7 +10728,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -12130,10 +11034,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E39"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -12141,8 +11045,8 @@
     <col min="1" max="1" width="15.125" style="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1"/>
     <col min="3" max="3" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" style="1"/>
-    <col min="5" max="5" width="14.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -12151,16 +11055,16 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -12168,19 +11072,19 @@
         <v>19</v>
       </c>
       <c r="B2" s="2">
-        <f t="shared" ref="B2:B37" si="0">C2/$C$39</f>
+        <f>C2/$E$2</f>
         <v>0.13680119762829629</v>
       </c>
       <c r="C2" s="1">
         <v>460014</v>
       </c>
-      <c r="D2" s="1">
-        <f>LOG(B2)</f>
-        <v>-0.86391010056119699</v>
-      </c>
-      <c r="E2" s="2">
+      <c r="D2" s="2">
         <f>SUM(B2:$B$37)</f>
         <v>1.0000000000000002</v>
+      </c>
+      <c r="E2" s="1">
+        <f>SUM(C2:$C$37)</f>
+        <v>3362646</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -12188,19 +11092,19 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B3:B37" si="0">C3/$E$2</f>
         <v>0.11258633825862134</v>
       </c>
       <c r="C3" s="1">
         <v>378588</v>
       </c>
-      <c r="D3" s="1">
-        <f t="shared" ref="D3:D37" si="1">LOG(B3)</f>
-        <v>-0.94851430556692251</v>
-      </c>
-      <c r="E3" s="2">
+      <c r="D3" s="2">
         <f>SUM(B3:$B$37)</f>
         <v>0.86319880237170388</v>
+      </c>
+      <c r="E3" s="1">
+        <f>SUM(C3:$C$37)</f>
+        <v>2902632</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -12214,13 +11118,13 @@
       <c r="C4" s="1">
         <v>230051</v>
       </c>
-      <c r="D4" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.164857024276589</v>
-      </c>
-      <c r="E4" s="2">
+      <c r="D4" s="2">
         <f>SUM(B4:$B$37)</f>
         <v>0.75061246411308258</v>
+      </c>
+      <c r="E4" s="1">
+        <f>SUM(C4:$C$37)</f>
+        <v>2524044</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -12234,13 +11138,13 @@
       <c r="C5" s="1">
         <v>228509</v>
       </c>
-      <c r="D5" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.167777839940024</v>
-      </c>
-      <c r="E5" s="2">
+      <c r="D5" s="2">
         <f>SUM(B5:$B$37)</f>
         <v>0.68219878036522441</v>
+      </c>
+      <c r="E5" s="1">
+        <f>SUM(C5:$C$37)</f>
+        <v>2293993</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -12254,13 +11158,13 @@
       <c r="C6" s="1">
         <v>223538</v>
       </c>
-      <c r="D6" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.1773297887306382</v>
-      </c>
-      <c r="E6" s="2">
+      <c r="D6" s="2">
         <f>SUM(B6:$B$37)</f>
         <v>0.61424366406692832</v>
+      </c>
+      <c r="E6" s="1">
+        <f>SUM(C6:$C$37)</f>
+        <v>2065484</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -12274,13 +11178,13 @@
       <c r="C7" s="1">
         <v>174178</v>
       </c>
-      <c r="D7" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.2856878502450029</v>
-      </c>
-      <c r="E7" s="2">
+      <c r="D7" s="2">
         <f>SUM(B7:$B$37)</f>
         <v>0.54776684789299857</v>
+      </c>
+      <c r="E7" s="1">
+        <f>SUM(C7:$C$37)</f>
+        <v>1841946</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -12294,13 +11198,13 @@
       <c r="C8" s="1">
         <v>173834</v>
       </c>
-      <c r="D8" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.2865464261011932</v>
-      </c>
-      <c r="E8" s="2">
+      <c r="D8" s="2">
         <f>SUM(B8:$B$37)</f>
         <v>0.49596894826276688</v>
+      </c>
+      <c r="E8" s="1">
+        <f>SUM(C8:$C$37)</f>
+        <v>1667768</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -12314,13 +11218,13 @@
       <c r="C9" s="1">
         <v>143452</v>
       </c>
-      <c r="D9" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.3699745421654546</v>
-      </c>
-      <c r="E9" s="2">
+      <c r="D9" s="2">
         <f>SUM(B9:$B$37)</f>
         <v>0.44427334902335841</v>
+      </c>
+      <c r="E9" s="1">
+        <f>SUM(C9:$C$37)</f>
+        <v>1493934</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -12334,13 +11238,13 @@
       <c r="C10" s="1">
         <v>141067</v>
       </c>
-      <c r="D10" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.3772557191778327</v>
-      </c>
-      <c r="E10" s="2">
+      <c r="D10" s="2">
         <f>SUM(B10:$B$37)</f>
         <v>0.40161289651066451</v>
+      </c>
+      <c r="E10" s="1">
+        <f>SUM(C10:$C$37)</f>
+        <v>1350482</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -12354,13 +11258,13 @@
       <c r="C11" s="1">
         <v>139457</v>
       </c>
-      <c r="D11" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.382240831276454</v>
-      </c>
-      <c r="E11" s="2">
+      <c r="D11" s="2">
         <f>SUM(B11:$B$37)</f>
         <v>0.35966170688202087</v>
+      </c>
+      <c r="E11" s="1">
+        <f>SUM(C11:$C$37)</f>
+        <v>1209415</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -12374,13 +11278,13 @@
       <c r="C12" s="1">
         <v>136429</v>
       </c>
-      <c r="D12" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.3917744538565757</v>
-      </c>
-      <c r="E12" s="2">
+      <c r="D12" s="2">
         <f>SUM(B12:$B$37)</f>
         <v>0.31818930687321828</v>
+      </c>
+      <c r="E12" s="1">
+        <f>SUM(C12:$C$37)</f>
+        <v>1069958</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -12394,13 +11298,13 @@
       <c r="C13" s="1">
         <v>119194</v>
       </c>
-      <c r="D13" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.4504267553062604</v>
-      </c>
-      <c r="E13" s="2">
+      <c r="D13" s="2">
         <f>SUM(B13:$B$37)</f>
         <v>0.27761738821154525</v>
+      </c>
+      <c r="E13" s="1">
+        <f>SUM(C13:$C$37)</f>
+        <v>933529</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -12414,13 +11318,13 @@
       <c r="C14" s="1">
         <v>111040</v>
       </c>
-      <c r="D14" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.481201696589002</v>
-      </c>
-      <c r="E14" s="2">
+      <c r="D14" s="2">
         <f>SUM(B14:$B$37)</f>
         <v>0.2421708975610278</v>
+      </c>
+      <c r="E14" s="1">
+        <f>SUM(C14:$C$37)</f>
+        <v>814335</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -12434,13 +11338,13 @@
       <c r="C15" s="1">
         <v>95547</v>
       </c>
-      <c r="D15" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.5464640941423404</v>
-      </c>
-      <c r="E15" s="2">
+      <c r="D15" s="2">
         <f>SUM(B15:$B$37)</f>
         <v>0.20914928303484814</v>
+      </c>
+      <c r="E15" s="1">
+        <f>SUM(C15:$C$37)</f>
+        <v>703295</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -12454,13 +11358,13 @@
       <c r="C16" s="1">
         <v>80487</v>
       </c>
-      <c r="D16" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.6209554095081635</v>
-      </c>
-      <c r="E16" s="2">
+      <c r="D16" s="2">
         <f>SUM(B16:$B$37)</f>
         <v>0.1807350520988531</v>
+      </c>
+      <c r="E16" s="1">
+        <f>SUM(C16:$C$37)</f>
+        <v>607748</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -12474,13 +11378,13 @@
       <c r="C17" s="1">
         <v>75077</v>
       </c>
-      <c r="D17" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.6511742393663003</v>
-      </c>
-      <c r="E17" s="2">
+      <c r="D17" s="2">
         <f>SUM(B17:$B$37)</f>
         <v>0.15679943710994257</v>
+      </c>
+      <c r="E17" s="1">
+        <f>SUM(C17:$C$37)</f>
+        <v>527261</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -12494,13 +11398,13 @@
       <c r="C18" s="1">
         <v>74618</v>
       </c>
-      <c r="D18" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.6538375453139769</v>
-      </c>
-      <c r="E18" s="2">
+      <c r="D18" s="2">
         <f>SUM(B18:$B$37)</f>
         <v>0.13447267419764078</v>
+      </c>
+      <c r="E18" s="1">
+        <f>SUM(C18:$C$37)</f>
+        <v>452184</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -12514,13 +11418,13 @@
       <c r="C19" s="1">
         <v>66485</v>
       </c>
-      <c r="D19" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.7039574766079217</v>
-      </c>
-      <c r="E19" s="2">
+      <c r="D19" s="2">
         <f>SUM(B19:$B$37)</f>
         <v>0.11228241093472223</v>
+      </c>
+      <c r="E19" s="1">
+        <f>SUM(C19:$C$37)</f>
+        <v>377566</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -12534,13 +11438,13 @@
       <c r="C20" s="1">
         <v>56131</v>
       </c>
-      <c r="D20" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.7774783702520085</v>
-      </c>
-      <c r="E20" s="2">
+      <c r="D20" s="2">
         <f>SUM(B20:$B$37)</f>
         <v>9.2510778714143579E-2</v>
+      </c>
+      <c r="E20" s="1">
+        <f>SUM(C20:$C$37)</f>
+        <v>311081</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -12554,13 +11458,13 @@
       <c r="C21" s="1">
         <v>40807</v>
       </c>
-      <c r="D21" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.9159464816929026</v>
-      </c>
-      <c r="E21" s="2">
+      <c r="D21" s="2">
         <f>SUM(B21:$B$37)</f>
         <v>7.5818269303399771E-2</v>
+      </c>
+      <c r="E21" s="1">
+        <f>SUM(C21:$C$37)</f>
+        <v>254950</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -12574,13 +11478,13 @@
       <c r="C22" s="1">
         <v>40674</v>
       </c>
-      <c r="D22" s="1">
-        <f t="shared" si="1"/>
-        <v>-1.9173642654066956</v>
-      </c>
-      <c r="E22" s="2">
+      <c r="D22" s="2">
         <f>SUM(B22:$B$37)</f>
         <v>6.3682885442000153E-2</v>
+      </c>
+      <c r="E22" s="1">
+        <f>SUM(C22:$C$37)</f>
+        <v>214143</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -12594,13 +11498,13 @@
       <c r="C23" s="1">
         <v>27755</v>
       </c>
-      <c r="D23" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.0833399180319021</v>
-      </c>
-      <c r="E23" s="2">
+      <c r="D23" s="2">
         <f>SUM(B23:$B$37)</f>
         <v>5.1587053766587398E-2</v>
+      </c>
+      <c r="E23" s="1">
+        <f>SUM(C23:$C$37)</f>
+        <v>173469</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -12614,13 +11518,13 @@
       <c r="C24" s="1">
         <v>25827</v>
       </c>
-      <c r="D24" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.1146071871622611</v>
-      </c>
-      <c r="E24" s="2">
+      <c r="D24" s="2">
         <f>SUM(B24:$B$37)</f>
         <v>4.3333137059327696E-2</v>
+      </c>
+      <c r="E24" s="1">
+        <f>SUM(C24:$C$37)</f>
+        <v>145714</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -12634,13 +11538,13 @@
       <c r="C25" s="1">
         <v>24415</v>
       </c>
-      <c r="D25" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.1390244210796396</v>
-      </c>
-      <c r="E25" s="2">
+      <c r="D25" s="2">
         <f>SUM(B25:$B$37)</f>
         <v>3.5652578356449062E-2</v>
+      </c>
+      <c r="E25" s="1">
+        <f>SUM(C25:$C$37)</f>
+        <v>119887</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -12654,13 +11558,13 @@
       <c r="C26" s="1">
         <v>15478</v>
       </c>
-      <c r="D26" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.3369663073761018</v>
-      </c>
-      <c r="E26" s="2">
+      <c r="D26" s="2">
         <f>SUM(B26:$B$37)</f>
         <v>2.8391927071716734E-2</v>
+      </c>
+      <c r="E26" s="1">
+        <f>SUM(C26:$C$37)</f>
+        <v>95472</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -12674,13 +11578,13 @@
       <c r="C27" s="1">
         <v>15069</v>
       </c>
-      <c r="D27" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.3485967168205701</v>
-      </c>
-      <c r="E27" s="2">
+      <c r="D27" s="2">
         <f>SUM(B27:$B$37)</f>
         <v>2.3789004254387763E-2</v>
+      </c>
+      <c r="E27" s="1">
+        <f>SUM(C27:$C$37)</f>
+        <v>79994</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -12694,13 +11598,13 @@
       <c r="C28" s="1">
         <v>12114</v>
       </c>
-      <c r="D28" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.4433935803724989</v>
-      </c>
-      <c r="E28" s="2">
+      <c r="D28" s="2">
         <f>SUM(B28:$B$37)</f>
         <v>1.9307711843589839E-2</v>
+      </c>
+      <c r="E28" s="1">
+        <f>SUM(C28:$C$37)</f>
+        <v>64925</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -12714,13 +11618,13 @@
       <c r="C29" s="1">
         <v>10465</v>
       </c>
-      <c r="D29" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.5069419170250766</v>
-      </c>
-      <c r="E29" s="2">
+      <c r="D29" s="2">
         <f>SUM(B29:$B$37)</f>
         <v>1.5705191685357302E-2</v>
+      </c>
+      <c r="E29" s="1">
+        <f>SUM(C29:$C$37)</f>
+        <v>52811</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -12734,13 +11638,13 @@
       <c r="C30" s="1">
         <v>8427</v>
       </c>
-      <c r="D30" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.6010081557785414</v>
-      </c>
-      <c r="E30" s="2">
+      <c r="D30" s="2">
         <f>SUM(B30:$B$37)</f>
         <v>1.2593059156390533E-2</v>
+      </c>
+      <c r="E30" s="1">
+        <f>SUM(C30:$C$37)</f>
+        <v>42346</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -12754,13 +11658,13 @@
       <c r="C31" s="1">
         <v>7008</v>
       </c>
-      <c r="D31" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.6810870565397575</v>
-      </c>
-      <c r="E31" s="2">
+      <c r="D31" s="2">
         <f>SUM(B31:$B$37)</f>
         <v>1.0086996966079688E-2</v>
+      </c>
+      <c r="E31" s="1">
+        <f>SUM(C31:$C$37)</f>
+        <v>33919</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -12774,13 +11678,13 @@
       <c r="C32" s="1">
         <v>6027</v>
       </c>
-      <c r="D32" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.74657995823187</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="D32" s="2">
         <f>SUM(B32:$B$37)</f>
         <v>8.0029238879144576E-3</v>
+      </c>
+      <c r="E32" s="1">
+        <f>SUM(C32:$C$37)</f>
+        <v>26911</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -12794,13 +11698,13 @@
       <c r="C33" s="1">
         <v>5703</v>
       </c>
-      <c r="D33" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.7705777781146761</v>
-      </c>
-      <c r="E33" s="2">
+      <c r="D33" s="2">
         <f>SUM(B33:$B$37)</f>
         <v>6.210585354509514E-3</v>
+      </c>
+      <c r="E33" s="1">
+        <f>SUM(C33:$C$37)</f>
+        <v>20884</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -12814,13 +11718,13 @@
       <c r="C34" s="1">
         <v>5497</v>
       </c>
-      <c r="D34" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.7865554127340513</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="D34" s="2">
         <f>SUM(B34:$B$37)</f>
         <v>4.514599514786867E-3</v>
+      </c>
+      <c r="E34" s="1">
+        <f>SUM(C34:$C$37)</f>
+        <v>15181</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -12834,13 +11738,13 @@
       <c r="C35" s="1">
         <v>4952</v>
       </c>
-      <c r="D35" s="1">
-        <f t="shared" si="1"/>
-        <v>-2.83190051368772</v>
-      </c>
-      <c r="E35" s="2">
+      <c r="D35" s="2">
         <f>SUM(B35:$B$37)</f>
         <v>2.8798749556153101E-3</v>
+      </c>
+      <c r="E35" s="1">
+        <f>SUM(C35:$C$37)</f>
+        <v>9684</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -12854,13 +11758,13 @@
       <c r="C36" s="1">
         <v>3119</v>
       </c>
-      <c r="D36" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.0326657749426378</v>
-      </c>
-      <c r="E36" s="2">
+      <c r="D36" s="2">
         <f>SUM(B36:$B$37)</f>
         <v>1.4072251435328013E-3</v>
+      </c>
+      <c r="E36" s="1">
+        <f>SUM(C36:$C$37)</f>
+        <v>4732</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -12874,22 +11778,13 @@
       <c r="C37" s="1">
         <v>1613</v>
       </c>
-      <c r="D37" s="1">
-        <f t="shared" si="1"/>
-        <v>-3.3190467823108203</v>
-      </c>
-      <c r="E37" s="2">
+      <c r="D37" s="2">
         <f>SUM(B37:$B$37)</f>
         <v>4.7968177441217423E-4</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C39" s="1">
-        <f>SUM(C2:C37)</f>
-        <v>3362646</v>
+      <c r="E37" s="1">
+        <f>SUM(C37:$C$37)</f>
+        <v>1613</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add unique token analysis, change grouping
</commit_message>
<xml_diff>
--- a/prefix_analysis.xlsx
+++ b/prefix_analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Cloud_Drive\Codes\Github_Repos\DSA_Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94068165-74B0-4A37-AD81-AB1C9183AE11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238356A0-6155-49AE-A079-2ECE0C13FC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -302,7 +302,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="39">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -514,7 +514,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -763,7 +787,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -789,6 +813,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="38" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="40" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="41" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="42" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -941,7 +977,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>t</c:v>
+                  <c:v>s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1036,12 +1072,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$2</c:f>
+              <c:f>prefix_result!$C$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.13680119762829629</c:v>
+                  <c:v>9.0231314743994359E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1061,7 +1097,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>a</c:v>
+                  <c:v>c</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1156,12 +1192,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$3</c:f>
+              <c:f>prefix_result!$C$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.11258633825862134</c:v>
+                  <c:v>7.4072698919541088E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1181,7 +1217,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s</c:v>
+                  <c:v>m</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1276,12 +1312,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$4</c:f>
+              <c:f>prefix_result!$C$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.8413683747858084E-2</c:v>
+                  <c:v>6.3216128912486541E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1301,7 +1337,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>o</c:v>
+                  <c:v>p</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1396,12 +1432,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$5</c:f>
+              <c:f>prefix_result!$C$5</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.795511629829605E-2</c:v>
+                  <c:v>6.0847287713956859E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1421,7 +1457,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>i</c:v>
+                  <c:v>a</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1516,12 +1552,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$6</c:f>
+              <c:f>prefix_result!$C$6</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.6476816173929698E-2</c:v>
+                  <c:v>5.8381910667211226E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1541,7 +1577,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>c</c:v>
+                  <c:v>b</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1636,12 +1672,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$7</c:f>
+              <c:f>prefix_result!$C$7</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.1797899630231667E-2</c:v>
+                  <c:v>5.6971002116362829E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1661,7 +1697,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>w</c:v>
+                  <c:v>t</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1756,12 +1792,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$8</c:f>
+              <c:f>prefix_result!$C$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.1695599239408488E-2</c:v>
+                  <c:v>4.5438681171796683E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1781,7 +1817,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>b</c:v>
+                  <c:v>d</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1876,12 +1912,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$9</c:f>
+              <c:f>prefix_result!$C$9</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.2660452512693875E-2</c:v>
+                  <c:v>4.4733226896372477E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1901,7 +1937,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p</c:v>
+                  <c:v>r</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1996,12 +2032,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$10</c:f>
+              <c:f>prefix_result!$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.1951189628643637E-2</c:v>
+                  <c:v>4.4116882634686071E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2021,7 +2057,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>f</c:v>
+                  <c:v>h</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2116,12 +2152,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$11</c:f>
+              <c:f>prefix_result!$C$11</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.147240000880259E-2</c:v>
+                  <c:v>3.6921249025359225E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2141,7 +2177,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>h</c:v>
+                  <c:v>g</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2236,12 +2272,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$12</c:f>
+              <c:f>prefix_result!$C$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.0571918661672979E-2</c:v>
+                  <c:v>3.5235584598819293E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2261,7 +2297,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>m</c:v>
+                  <c:v>l</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2356,12 +2392,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$13</c:f>
+              <c:f>prefix_result!$C$13</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.5446490650517477E-2</c:v>
+                  <c:v>3.3438532655107114E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2381,7 +2417,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>r</c:v>
+                  <c:v>k</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2476,12 +2512,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$14</c:f>
+              <c:f>prefix_result!$C$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.3021614526179681E-2</c:v>
+                  <c:v>3.2257824973081349E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2501,7 +2537,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>d</c:v>
+                  <c:v>f</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2596,12 +2632,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$15</c:f>
+              <c:f>prefix_result!$C$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.8414230935995047E-2</c:v>
+                  <c:v>3.1544944863178999E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2621,7 +2657,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>l</c:v>
+                  <c:v>e</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2716,12 +2752,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$16</c:f>
+              <c:f>prefix_result!$C$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.393561498891052E-2</c:v>
+                  <c:v>3.1329595663312663E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2836,12 +2872,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$17</c:f>
+              <c:f>prefix_result!$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.23267629123018E-2</c:v>
+                  <c:v>2.7906285968885752E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2861,7 +2897,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>e</c:v>
+                  <c:v>i</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2956,12 +2992,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$18</c:f>
+              <c:f>prefix_result!$C$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.2190263262918546E-2</c:v>
+                  <c:v>2.7223109196896002E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3076,12 +3112,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$19</c:f>
+              <c:f>prefix_result!$C$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.9771632220578674E-2</c:v>
+                  <c:v>2.6978056659117067E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3101,7 +3137,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>g</c:v>
+                  <c:v>w</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3196,12 +3232,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$20</c:f>
+              <c:f>prefix_result!$C$20</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.6692509410743801E-2</c:v>
+                  <c:v>2.322801024765158E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3221,7 +3257,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>u</c:v>
+                  <c:v>o</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3316,12 +3352,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$21</c:f>
+              <c:f>prefix_result!$C$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.2135383861399625E-2</c:v>
+                  <c:v>1.9708164705008725E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3341,7 +3377,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>v</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3436,12 +3472,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$22</c:f>
+              <c:f>prefix_result!$C$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.2095831675412755E-2</c:v>
+                  <c:v>1.86239928711989E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3461,7 +3497,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v</c:v>
+                  <c:v>u</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3556,12 +3592,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$23</c:f>
+              <c:f>prefix_result!$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8.2539167072597005E-3</c:v>
+                  <c:v>1.4977908142427505E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3676,12 +3712,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$24</c:f>
+              <c:f>prefix_result!$C$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7.6805587028786256E-3</c:v>
+                  <c:v>1.3373927895147217E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3701,7 +3737,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>k</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3796,12 +3832,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$25</c:f>
+              <c:f>prefix_result!$C$25</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7.260651284732321E-3</c:v>
+                  <c:v>1.161400512382579E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3821,7 +3857,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3916,12 +3952,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$26</c:f>
+              <c:f>prefix_result!$C$26</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.6029228173289725E-3</c:v>
+                  <c:v>9.4902164630750376E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4036,12 +4072,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$27</c:f>
+              <c:f>prefix_result!$C$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.4812924107979256E-3</c:v>
+                  <c:v>9.2525897597742542E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4061,7 +4097,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4140,12 +4176,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$28</c:f>
+              <c:f>prefix_result!$C$28</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.6025201582325348E-3</c:v>
+                  <c:v>8.8367430289978833E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4165,7 +4201,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4244,12 +4280,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$29</c:f>
+              <c:f>prefix_result!$C$29</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.112132528966772E-3</c:v>
+                  <c:v>7.1585044369361006E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4269,7 +4305,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>y</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4348,12 +4384,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$30</c:f>
+              <c:f>prefix_result!$C$30</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.5060621903108446E-3</c:v>
+                  <c:v>6.6386960234656369E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4373,7 +4409,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4452,12 +4488,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$31</c:f>
+              <c:f>prefix_result!$C$31</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.0840730781652305E-3</c:v>
+                  <c:v>6.5644376786841421E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4477,7 +4513,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>z</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4556,12 +4592,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$32</c:f>
+              <c:f>prefix_result!$C$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.7923385334049436E-3</c:v>
+                  <c:v>6.2971076374707608E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4581,7 +4617,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4660,12 +4696,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$33</c:f>
+              <c:f>prefix_result!$C$33</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.695985839722647E-3</c:v>
+                  <c:v>5.9183900790851368E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4764,12 +4800,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$34</c:f>
+              <c:f>prefix_result!$C$34</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.6347245591715571E-3</c:v>
+                  <c:v>5.6362083689154565E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4789,7 +4825,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>q</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4868,12 +4904,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$35</c:f>
+              <c:f>prefix_result!$C$35</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.4726498120825088E-3</c:v>
+                  <c:v>5.5025433483087659E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4893,7 +4929,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>q</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4972,12 +5008,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$36</c:f>
+              <c:f>prefix_result!$C$36</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.2754336912062704E-4</c:v>
+                  <c:v>4.0619314595477666E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5076,12 +5112,12 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>prefix_result!$B$37</c:f>
+              <c:f>prefix_result!$C$37</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.7968177441217423E-4</c:v>
+                  <c:v>2.2723053503137416E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5340,7 +5376,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>t</c:v>
+                  <c:v>s</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5440,7 +5476,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.0000000000000002</c:v>
+                  <c:v>0.99999999999999989</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5460,7 +5496,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>a</c:v>
+                  <c:v>c</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5560,7 +5596,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.86319880237170388</c:v>
+                  <c:v>0.90976868525600552</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5580,7 +5616,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>s</c:v>
+                  <c:v>m</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5680,7 +5716,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.75061246411308258</c:v>
+                  <c:v>0.83569598633646447</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5700,7 +5736,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>o</c:v>
+                  <c:v>p</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5800,7 +5836,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.68219878036522441</c:v>
+                  <c:v>0.77247985742397784</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5820,7 +5856,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>i</c:v>
+                  <c:v>a</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -5920,7 +5956,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.61424366406692832</c:v>
+                  <c:v>0.71163256971002109</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5940,7 +5976,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>c</c:v>
+                  <c:v>b</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6040,7 +6076,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.54776684789299857</c:v>
+                  <c:v>0.65325065904280988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6060,7 +6096,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>w</c:v>
+                  <c:v>t</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6160,7 +6196,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.49596894826276688</c:v>
+                  <c:v>0.59627965692644713</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6180,7 +6216,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>b</c:v>
+                  <c:v>d</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6280,7 +6316,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.44427334902335841</c:v>
+                  <c:v>0.55084097575465041</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6300,7 +6336,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>p</c:v>
+                  <c:v>r</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6400,7 +6436,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.40161289651066451</c:v>
+                  <c:v>0.50610774885827803</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6420,7 +6456,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>f</c:v>
+                  <c:v>h</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6520,7 +6556,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.35966170688202087</c:v>
+                  <c:v>0.46199086622359187</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6540,7 +6576,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>h</c:v>
+                  <c:v>g</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6640,7 +6676,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.31818930687321828</c:v>
+                  <c:v>0.42506961719823261</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6660,7 +6696,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>m</c:v>
+                  <c:v>l</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6760,7 +6796,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.27761738821154525</c:v>
+                  <c:v>0.38983403259941329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6780,7 +6816,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>r</c:v>
+                  <c:v>k</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -6880,7 +6916,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.2421708975610278</c:v>
+                  <c:v>0.35639549994430619</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6900,7 +6936,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>d</c:v>
+                  <c:v>f</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7000,7 +7036,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.20914928303484814</c:v>
+                  <c:v>0.32413767497122481</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7020,7 +7056,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>l</c:v>
+                  <c:v>e</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7120,7 +7156,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.1807350520988531</c:v>
+                  <c:v>0.29259273010804582</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7240,7 +7276,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.15679943710994257</c:v>
+                  <c:v>0.26126313444473326</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7260,7 +7296,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>e</c:v>
+                  <c:v>i</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7360,7 +7396,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.13447267419764078</c:v>
+                  <c:v>0.23335684847584751</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7480,7 +7516,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.11228241093472223</c:v>
+                  <c:v>0.20613373927895154</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7500,7 +7536,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>g</c:v>
+                  <c:v>w</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7600,7 +7636,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>9.2510778714143579E-2</c:v>
+                  <c:v>0.17915568261983442</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7620,7 +7656,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>u</c:v>
+                  <c:v>o</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7720,7 +7756,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7.5818269303399771E-2</c:v>
+                  <c:v>0.15592767237218283</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7740,7 +7776,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>v</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7840,7 +7876,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.3682885442000153E-2</c:v>
+                  <c:v>0.13621950766717411</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7860,7 +7896,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>v</c:v>
+                  <c:v>u</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -7960,7 +7996,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5.1587053766587398E-2</c:v>
+                  <c:v>0.1175955147959752</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8080,7 +8116,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.3333137059327696E-2</c:v>
+                  <c:v>0.1026176066535477</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8100,7 +8136,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>k</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8200,7 +8236,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>3.5652578356449062E-2</c:v>
+                  <c:v>8.9243678758400474E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8220,7 +8256,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>y</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8320,7 +8356,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.8391927071716734E-2</c:v>
+                  <c:v>7.7629673634574681E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8440,7 +8476,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.3789004254387763E-2</c:v>
+                  <c:v>6.8139457171499648E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8460,7 +8496,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8544,7 +8580,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.9307711843589839E-2</c:v>
+                  <c:v>5.8886867411725385E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8564,7 +8600,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8648,7 +8684,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.5705191685357302E-2</c:v>
+                  <c:v>5.0050124382727504E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8668,7 +8704,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6</c:v>
+                  <c:v>y</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8752,7 +8788,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.2593059156390533E-2</c:v>
+                  <c:v>4.2891619945791402E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8772,7 +8808,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8856,7 +8892,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.0086996966079688E-2</c:v>
+                  <c:v>3.6252923922325771E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8876,7 +8912,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8</c:v>
+                  <c:v>z</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -8960,7 +8996,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>8.0029238879144576E-3</c:v>
+                  <c:v>2.9688486243641628E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8980,7 +9016,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9064,7 +9100,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>6.210585354509514E-3</c:v>
+                  <c:v>2.3391378606170868E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9168,7 +9204,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.514599514786867E-3</c:v>
+                  <c:v>1.7472988527085731E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9188,7 +9224,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>q</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9272,7 +9308,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>2.8798749556153101E-3</c:v>
+                  <c:v>1.1836780158170274E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9292,7 +9328,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>z</c:v>
+                  <c:v>q</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -9376,7 +9412,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>1.4072251435328013E-3</c:v>
+                  <c:v>6.3342368098615077E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -9480,7 +9516,7 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.7968177441217423E-4</c:v>
+                  <c:v>2.2723053503137416E-3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11034,20 +11070,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1"/>
-    <col min="3" max="3" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="1"/>
     <col min="4" max="4" width="14.125" style="1" customWidth="1"/>
     <col min="5" max="5" width="15.625" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9" style="1"/>
+    <col min="7" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -11055,10 +11091,10 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>29</v>
@@ -11068,728 +11104,728 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="2">
-        <f>C2/$E$2</f>
-        <v>0.13680119762829629</v>
-      </c>
-      <c r="C2" s="1">
-        <v>460014</v>
+      <c r="A2" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="1">
+        <v>12151</v>
+      </c>
+      <c r="C2" s="2">
+        <f>B2/$E$2</f>
+        <v>9.0231314743994359E-2</v>
       </c>
       <c r="D2" s="2">
+        <f>SUM(C2:$C$37)</f>
+        <v>0.99999999999999989</v>
+      </c>
+      <c r="E2" s="1">
         <f>SUM(B2:$B$37)</f>
-        <v>1.0000000000000002</v>
-      </c>
-      <c r="E2" s="1">
-        <f>SUM(C2:$C$37)</f>
-        <v>3362646</v>
+        <v>134665</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2">
-        <f t="shared" ref="B3:B37" si="0">C3/$E$2</f>
-        <v>0.11258633825862134</v>
-      </c>
-      <c r="C3" s="1">
-        <v>378588</v>
+      <c r="A3" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>9975</v>
+      </c>
+      <c r="C3" s="2">
+        <f>B3/$E$2</f>
+        <v>7.4072698919541088E-2</v>
       </c>
       <c r="D3" s="2">
+        <f>SUM(C3:$C$37)</f>
+        <v>0.90976868525600552</v>
+      </c>
+      <c r="E3" s="1">
         <f>SUM(B3:$B$37)</f>
-        <v>0.86319880237170388</v>
-      </c>
-      <c r="E3" s="1">
-        <f>SUM(C3:$C$37)</f>
-        <v>2902632</v>
+        <v>122514</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2">
-        <f t="shared" si="0"/>
-        <v>6.8413683747858084E-2</v>
-      </c>
-      <c r="C4" s="1">
-        <v>230051</v>
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8513</v>
+      </c>
+      <c r="C4" s="2">
+        <f>B4/$E$2</f>
+        <v>6.3216128912486541E-2</v>
       </c>
       <c r="D4" s="2">
+        <f>SUM(C4:$C$37)</f>
+        <v>0.83569598633646447</v>
+      </c>
+      <c r="E4" s="1">
         <f>SUM(B4:$B$37)</f>
-        <v>0.75061246411308258</v>
-      </c>
-      <c r="E4" s="1">
-        <f>SUM(C4:$C$37)</f>
-        <v>2524044</v>
+        <v>112539</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="2">
-        <f t="shared" si="0"/>
-        <v>6.795511629829605E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <v>228509</v>
+      <c r="A5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8194</v>
+      </c>
+      <c r="C5" s="2">
+        <f>B5/$E$2</f>
+        <v>6.0847287713956859E-2</v>
       </c>
       <c r="D5" s="2">
+        <f>SUM(C5:$C$37)</f>
+        <v>0.77247985742397784</v>
+      </c>
+      <c r="E5" s="1">
         <f>SUM(B5:$B$37)</f>
-        <v>0.68219878036522441</v>
-      </c>
-      <c r="E5" s="1">
-        <f>SUM(C5:$C$37)</f>
-        <v>2293993</v>
+        <v>104026</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <f t="shared" si="0"/>
-        <v>6.6476816173929698E-2</v>
-      </c>
-      <c r="C6" s="1">
-        <v>223538</v>
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1">
+        <v>7862</v>
+      </c>
+      <c r="C6" s="2">
+        <f>B6/$E$2</f>
+        <v>5.8381910667211226E-2</v>
       </c>
       <c r="D6" s="2">
+        <f>SUM(C6:$C$37)</f>
+        <v>0.71163256971002109</v>
+      </c>
+      <c r="E6" s="1">
         <f>SUM(B6:$B$37)</f>
-        <v>0.61424366406692832</v>
-      </c>
-      <c r="E6" s="1">
-        <f>SUM(C6:$C$37)</f>
-        <v>2065484</v>
+        <v>95832</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="2">
-        <f t="shared" si="0"/>
-        <v>5.1797899630231667E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>174178</v>
+      <c r="A7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7672</v>
+      </c>
+      <c r="C7" s="2">
+        <f>B7/$E$2</f>
+        <v>5.6971002116362829E-2</v>
       </c>
       <c r="D7" s="2">
+        <f>SUM(C7:$C$37)</f>
+        <v>0.65325065904280988</v>
+      </c>
+      <c r="E7" s="1">
         <f>SUM(B7:$B$37)</f>
-        <v>0.54776684789299857</v>
-      </c>
-      <c r="E7" s="1">
-        <f>SUM(C7:$C$37)</f>
-        <v>1841946</v>
+        <v>87970</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="2">
-        <f t="shared" si="0"/>
-        <v>5.1695599239408488E-2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>173834</v>
+      <c r="A8" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6119</v>
+      </c>
+      <c r="C8" s="2">
+        <f>B8/$E$2</f>
+        <v>4.5438681171796683E-2</v>
       </c>
       <c r="D8" s="2">
+        <f>SUM(C8:$C$37)</f>
+        <v>0.59627965692644713</v>
+      </c>
+      <c r="E8" s="1">
         <f>SUM(B8:$B$37)</f>
-        <v>0.49596894826276688</v>
-      </c>
-      <c r="E8" s="1">
-        <f>SUM(C8:$C$37)</f>
-        <v>1667768</v>
+        <v>80298</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2">
-        <f t="shared" si="0"/>
-        <v>4.2660452512693875E-2</v>
-      </c>
-      <c r="C9" s="1">
-        <v>143452</v>
+      <c r="A9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>6024</v>
+      </c>
+      <c r="C9" s="2">
+        <f>B9/$E$2</f>
+        <v>4.4733226896372477E-2</v>
       </c>
       <c r="D9" s="2">
+        <f>SUM(C9:$C$37)</f>
+        <v>0.55084097575465041</v>
+      </c>
+      <c r="E9" s="1">
         <f>SUM(B9:$B$37)</f>
-        <v>0.44427334902335841</v>
-      </c>
-      <c r="E9" s="1">
-        <f>SUM(C9:$C$37)</f>
-        <v>1493934</v>
+        <v>74179</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="2">
-        <f t="shared" si="0"/>
-        <v>4.1951189628643637E-2</v>
-      </c>
-      <c r="C10" s="1">
-        <v>141067</v>
+      <c r="A10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="1">
+        <v>5941</v>
+      </c>
+      <c r="C10" s="2">
+        <f>B10/$E$2</f>
+        <v>4.4116882634686071E-2</v>
       </c>
       <c r="D10" s="2">
+        <f>SUM(C10:$C$37)</f>
+        <v>0.50610774885827803</v>
+      </c>
+      <c r="E10" s="1">
         <f>SUM(B10:$B$37)</f>
-        <v>0.40161289651066451</v>
-      </c>
-      <c r="E10" s="1">
-        <f>SUM(C10:$C$37)</f>
-        <v>1350482</v>
+        <v>68155</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="2">
-        <f t="shared" si="0"/>
-        <v>4.147240000880259E-2</v>
-      </c>
-      <c r="C11" s="1">
-        <v>139457</v>
+      <c r="A11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1">
+        <v>4972</v>
+      </c>
+      <c r="C11" s="2">
+        <f>B11/$E$2</f>
+        <v>3.6921249025359225E-2</v>
       </c>
       <c r="D11" s="2">
+        <f>SUM(C11:$C$37)</f>
+        <v>0.46199086622359187</v>
+      </c>
+      <c r="E11" s="1">
         <f>SUM(B11:$B$37)</f>
-        <v>0.35966170688202087</v>
-      </c>
-      <c r="E11" s="1">
-        <f>SUM(C11:$C$37)</f>
-        <v>1209415</v>
+        <v>62214</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2">
-        <f t="shared" si="0"/>
-        <v>4.0571918661672979E-2</v>
-      </c>
-      <c r="C12" s="1">
-        <v>136429</v>
+      <c r="A12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>4745</v>
+      </c>
+      <c r="C12" s="2">
+        <f>B12/$E$2</f>
+        <v>3.5235584598819293E-2</v>
       </c>
       <c r="D12" s="2">
+        <f>SUM(C12:$C$37)</f>
+        <v>0.42506961719823261</v>
+      </c>
+      <c r="E12" s="1">
         <f>SUM(B12:$B$37)</f>
-        <v>0.31818930687321828</v>
-      </c>
-      <c r="E12" s="1">
-        <f>SUM(C12:$C$37)</f>
-        <v>1069958</v>
+        <v>57242</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="2">
-        <f t="shared" si="0"/>
-        <v>3.5446490650517477E-2</v>
-      </c>
-      <c r="C13" s="1">
-        <v>119194</v>
+      <c r="A13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1">
+        <v>4503</v>
+      </c>
+      <c r="C13" s="2">
+        <f>B13/$E$2</f>
+        <v>3.3438532655107114E-2</v>
       </c>
       <c r="D13" s="2">
+        <f>SUM(C13:$C$37)</f>
+        <v>0.38983403259941329</v>
+      </c>
+      <c r="E13" s="1">
         <f>SUM(B13:$B$37)</f>
-        <v>0.27761738821154525</v>
-      </c>
-      <c r="E13" s="1">
-        <f>SUM(C13:$C$37)</f>
-        <v>933529</v>
+        <v>52497</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="2">
-        <f t="shared" si="0"/>
-        <v>3.3021614526179681E-2</v>
-      </c>
-      <c r="C14" s="1">
-        <v>111040</v>
+      <c r="A14" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="1">
+        <v>4344</v>
+      </c>
+      <c r="C14" s="2">
+        <f>B14/$E$2</f>
+        <v>3.2257824973081349E-2</v>
       </c>
       <c r="D14" s="2">
+        <f>SUM(C14:$C$37)</f>
+        <v>0.35639549994430619</v>
+      </c>
+      <c r="E14" s="1">
         <f>SUM(B14:$B$37)</f>
-        <v>0.2421708975610278</v>
-      </c>
-      <c r="E14" s="1">
-        <f>SUM(C14:$C$37)</f>
-        <v>814335</v>
+        <v>47994</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2">
-        <f t="shared" si="0"/>
-        <v>2.8414230935995047E-2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>95547</v>
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="1">
+        <v>4248</v>
+      </c>
+      <c r="C15" s="2">
+        <f>B15/$E$2</f>
+        <v>3.1544944863178999E-2</v>
       </c>
       <c r="D15" s="2">
+        <f>SUM(C15:$C$37)</f>
+        <v>0.32413767497122481</v>
+      </c>
+      <c r="E15" s="1">
         <f>SUM(B15:$B$37)</f>
-        <v>0.20914928303484814</v>
-      </c>
-      <c r="E15" s="1">
-        <f>SUM(C15:$C$37)</f>
-        <v>703295</v>
+        <v>43650</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" s="2">
-        <f t="shared" si="0"/>
-        <v>2.393561498891052E-2</v>
-      </c>
-      <c r="C16" s="1">
-        <v>80487</v>
+      <c r="A16" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1">
+        <v>4219</v>
+      </c>
+      <c r="C16" s="2">
+        <f>B16/$E$2</f>
+        <v>3.1329595663312663E-2</v>
       </c>
       <c r="D16" s="2">
+        <f>SUM(C16:$C$37)</f>
+        <v>0.29259273010804582</v>
+      </c>
+      <c r="E16" s="1">
         <f>SUM(B16:$B$37)</f>
-        <v>0.1807350520988531</v>
-      </c>
-      <c r="E16" s="1">
-        <f>SUM(C16:$C$37)</f>
-        <v>607748</v>
+        <v>39402</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="2">
-        <f t="shared" si="0"/>
-        <v>2.23267629123018E-2</v>
-      </c>
-      <c r="C17" s="1">
-        <v>75077</v>
+      <c r="B17" s="1">
+        <v>3758</v>
+      </c>
+      <c r="C17" s="2">
+        <f>B17/$E$2</f>
+        <v>2.7906285968885752E-2</v>
       </c>
       <c r="D17" s="2">
+        <f>SUM(C17:$C$37)</f>
+        <v>0.26126313444473326</v>
+      </c>
+      <c r="E17" s="1">
         <f>SUM(B17:$B$37)</f>
-        <v>0.15679943710994257</v>
-      </c>
-      <c r="E17" s="1">
-        <f>SUM(C17:$C$37)</f>
-        <v>527261</v>
+        <v>35183</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B18" s="2">
-        <f t="shared" si="0"/>
-        <v>2.2190263262918546E-2</v>
-      </c>
-      <c r="C18" s="1">
-        <v>74618</v>
+      <c r="A18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="1">
+        <v>3666</v>
+      </c>
+      <c r="C18" s="2">
+        <f>B18/$E$2</f>
+        <v>2.7223109196896002E-2</v>
       </c>
       <c r="D18" s="2">
+        <f>SUM(C18:$C$37)</f>
+        <v>0.23335684847584751</v>
+      </c>
+      <c r="E18" s="1">
         <f>SUM(B18:$B$37)</f>
-        <v>0.13447267419764078</v>
-      </c>
-      <c r="E18" s="1">
-        <f>SUM(C18:$C$37)</f>
-        <v>452184</v>
+        <v>31425</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="2">
-        <f t="shared" si="0"/>
-        <v>1.9771632220578674E-2</v>
-      </c>
-      <c r="C19" s="1">
-        <v>66485</v>
+      <c r="B19" s="1">
+        <v>3633</v>
+      </c>
+      <c r="C19" s="2">
+        <f>B19/$E$2</f>
+        <v>2.6978056659117067E-2</v>
       </c>
       <c r="D19" s="2">
+        <f>SUM(C19:$C$37)</f>
+        <v>0.20613373927895154</v>
+      </c>
+      <c r="E19" s="1">
         <f>SUM(B19:$B$37)</f>
-        <v>0.11228241093472223</v>
-      </c>
-      <c r="E19" s="1">
-        <f>SUM(C19:$C$37)</f>
-        <v>377566</v>
+        <v>27759</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" s="2">
-        <f t="shared" si="0"/>
-        <v>1.6692509410743801E-2</v>
-      </c>
-      <c r="C20" s="1">
-        <v>56131</v>
+      <c r="A20" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>3128</v>
+      </c>
+      <c r="C20" s="2">
+        <f>B20/$E$2</f>
+        <v>2.322801024765158E-2</v>
       </c>
       <c r="D20" s="2">
+        <f>SUM(C20:$C$37)</f>
+        <v>0.17915568261983442</v>
+      </c>
+      <c r="E20" s="1">
         <f>SUM(B20:$B$37)</f>
-        <v>9.2510778714143579E-2</v>
-      </c>
-      <c r="E20" s="1">
-        <f>SUM(C20:$C$37)</f>
-        <v>311081</v>
+        <v>24126</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B21" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2135383861399625E-2</v>
-      </c>
-      <c r="C21" s="1">
-        <v>40807</v>
+      <c r="A21" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="1">
+        <v>2654</v>
+      </c>
+      <c r="C21" s="2">
+        <f>B21/$E$2</f>
+        <v>1.9708164705008725E-2</v>
       </c>
       <c r="D21" s="2">
+        <f>SUM(C21:$C$37)</f>
+        <v>0.15592767237218283</v>
+      </c>
+      <c r="E21" s="1">
         <f>SUM(B21:$B$37)</f>
-        <v>7.5818269303399771E-2</v>
-      </c>
-      <c r="E21" s="1">
-        <f>SUM(C21:$C$37)</f>
-        <v>254950</v>
+        <v>20998</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
-        <v>2</v>
-      </c>
-      <c r="B22" s="2">
-        <f t="shared" si="0"/>
-        <v>1.2095831675412755E-2</v>
-      </c>
-      <c r="C22" s="1">
-        <v>40674</v>
+      <c r="A22" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1">
+        <v>2508</v>
+      </c>
+      <c r="C22" s="2">
+        <f>B22/$E$2</f>
+        <v>1.86239928711989E-2</v>
       </c>
       <c r="D22" s="2">
+        <f>SUM(C22:$C$37)</f>
+        <v>0.13621950766717411</v>
+      </c>
+      <c r="E22" s="1">
         <f>SUM(B22:$B$37)</f>
-        <v>6.3682885442000153E-2</v>
-      </c>
-      <c r="E22" s="1">
-        <f>SUM(C22:$C$37)</f>
-        <v>214143</v>
+        <v>18344</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B23" s="2">
-        <f t="shared" si="0"/>
-        <v>8.2539167072597005E-3</v>
-      </c>
-      <c r="C23" s="1">
-        <v>27755</v>
+      <c r="A23" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" s="1">
+        <v>2017</v>
+      </c>
+      <c r="C23" s="2">
+        <f>B23/$E$2</f>
+        <v>1.4977908142427505E-2</v>
       </c>
       <c r="D23" s="2">
+        <f>SUM(C23:$C$37)</f>
+        <v>0.1175955147959752</v>
+      </c>
+      <c r="E23" s="1">
         <f>SUM(B23:$B$37)</f>
-        <v>5.1587053766587398E-2</v>
-      </c>
-      <c r="E23" s="1">
-        <f>SUM(C23:$C$37)</f>
-        <v>173469</v>
+        <v>15836</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="2">
-        <f t="shared" si="0"/>
-        <v>7.6805587028786256E-3</v>
-      </c>
-      <c r="C24" s="1">
-        <v>25827</v>
+      <c r="B24" s="1">
+        <v>1801</v>
+      </c>
+      <c r="C24" s="2">
+        <f>B24/$E$2</f>
+        <v>1.3373927895147217E-2</v>
       </c>
       <c r="D24" s="2">
+        <f>SUM(C24:$C$37)</f>
+        <v>0.1026176066535477</v>
+      </c>
+      <c r="E24" s="1">
         <f>SUM(B24:$B$37)</f>
-        <v>4.3333137059327696E-2</v>
-      </c>
-      <c r="E24" s="1">
-        <f>SUM(C24:$C$37)</f>
-        <v>145714</v>
+        <v>13819</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B25" s="2">
-        <f t="shared" si="0"/>
-        <v>7.260651284732321E-3</v>
-      </c>
-      <c r="C25" s="1">
-        <v>24415</v>
+      <c r="A25" s="9">
+        <v>2</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1564</v>
+      </c>
+      <c r="C25" s="2">
+        <f>B25/$E$2</f>
+        <v>1.161400512382579E-2</v>
       </c>
       <c r="D25" s="2">
+        <f>SUM(C25:$C$37)</f>
+        <v>8.9243678758400474E-2</v>
+      </c>
+      <c r="E25" s="1">
         <f>SUM(B25:$B$37)</f>
-        <v>3.5652578356449062E-2</v>
-      </c>
-      <c r="E25" s="1">
-        <f>SUM(C25:$C$37)</f>
-        <v>119887</v>
+        <v>12018</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B26" s="2">
-        <f t="shared" si="0"/>
-        <v>4.6029228173289725E-3</v>
-      </c>
-      <c r="C26" s="1">
-        <v>15478</v>
+      <c r="A26" s="9">
+        <v>4</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1278</v>
+      </c>
+      <c r="C26" s="2">
+        <f>B26/$E$2</f>
+        <v>9.4902164630750376E-3</v>
       </c>
       <c r="D26" s="2">
+        <f>SUM(C26:$C$37)</f>
+        <v>7.7629673634574681E-2</v>
+      </c>
+      <c r="E26" s="1">
         <f>SUM(B26:$B$37)</f>
-        <v>2.8391927071716734E-2</v>
-      </c>
-      <c r="E26" s="1">
-        <f>SUM(C26:$C$37)</f>
-        <v>95472</v>
+        <v>10454</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
+      <c r="A27" s="9">
         <v>3</v>
       </c>
-      <c r="B27" s="2">
-        <f t="shared" si="0"/>
-        <v>4.4812924107979256E-3</v>
-      </c>
-      <c r="C27" s="1">
-        <v>15069</v>
+      <c r="B27" s="1">
+        <v>1246</v>
+      </c>
+      <c r="C27" s="2">
+        <f>B27/$E$2</f>
+        <v>9.2525897597742542E-3</v>
       </c>
       <c r="D27" s="2">
+        <f>SUM(C27:$C$37)</f>
+        <v>6.8139457171499648E-2</v>
+      </c>
+      <c r="E27" s="1">
         <f>SUM(B27:$B$37)</f>
-        <v>2.3789004254387763E-2</v>
-      </c>
-      <c r="E27" s="1">
-        <f>SUM(C27:$C$37)</f>
-        <v>79994</v>
+        <v>9176</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="3">
-        <v>4</v>
-      </c>
-      <c r="B28" s="2">
-        <f t="shared" si="0"/>
-        <v>3.6025201582325348E-3</v>
-      </c>
-      <c r="C28" s="1">
-        <v>12114</v>
+      <c r="A28" s="9">
+        <v>5</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1190</v>
+      </c>
+      <c r="C28" s="2">
+        <f>B28/$E$2</f>
+        <v>8.8367430289978833E-3</v>
       </c>
       <c r="D28" s="2">
+        <f>SUM(C28:$C$37)</f>
+        <v>5.8886867411725385E-2</v>
+      </c>
+      <c r="E28" s="1">
         <f>SUM(B28:$B$37)</f>
-        <v>1.9307711843589839E-2</v>
-      </c>
-      <c r="E28" s="1">
-        <f>SUM(C28:$C$37)</f>
-        <v>64925</v>
+        <v>7930</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="3">
-        <v>5</v>
-      </c>
-      <c r="B29" s="2">
-        <f t="shared" si="0"/>
-        <v>3.112132528966772E-3</v>
-      </c>
-      <c r="C29" s="1">
-        <v>10465</v>
+      <c r="A29" s="8">
+        <v>7</v>
+      </c>
+      <c r="B29" s="1">
+        <v>964</v>
+      </c>
+      <c r="C29" s="2">
+        <f>B29/$E$2</f>
+        <v>7.1585044369361006E-3</v>
       </c>
       <c r="D29" s="2">
+        <f>SUM(C29:$C$37)</f>
+        <v>5.0050124382727504E-2</v>
+      </c>
+      <c r="E29" s="1">
         <f>SUM(B29:$B$37)</f>
-        <v>1.5705191685357302E-2</v>
-      </c>
-      <c r="E29" s="1">
-        <f>SUM(C29:$C$37)</f>
-        <v>52811</v>
+        <v>6740</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="3">
-        <v>6</v>
-      </c>
-      <c r="B30" s="2">
-        <f t="shared" si="0"/>
-        <v>2.5060621903108446E-3</v>
-      </c>
-      <c r="C30" s="1">
-        <v>8427</v>
+      <c r="A30" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B30" s="1">
+        <v>894</v>
+      </c>
+      <c r="C30" s="2">
+        <f>B30/$E$2</f>
+        <v>6.6386960234656369E-3</v>
       </c>
       <c r="D30" s="2">
+        <f>SUM(C30:$C$37)</f>
+        <v>4.2891619945791402E-2</v>
+      </c>
+      <c r="E30" s="1">
         <f>SUM(B30:$B$37)</f>
-        <v>1.2593059156390533E-2</v>
-      </c>
-      <c r="E30" s="1">
-        <f>SUM(C30:$C$37)</f>
-        <v>42346</v>
+        <v>5776</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="3">
-        <v>7</v>
-      </c>
-      <c r="B31" s="2">
-        <f t="shared" si="0"/>
-        <v>2.0840730781652305E-3</v>
-      </c>
-      <c r="C31" s="1">
-        <v>7008</v>
+      <c r="A31" s="8">
+        <v>6</v>
+      </c>
+      <c r="B31" s="1">
+        <v>884</v>
+      </c>
+      <c r="C31" s="2">
+        <f>B31/$E$2</f>
+        <v>6.5644376786841421E-3</v>
       </c>
       <c r="D31" s="2">
+        <f>SUM(C31:$C$37)</f>
+        <v>3.6252923922325771E-2</v>
+      </c>
+      <c r="E31" s="1">
         <f>SUM(B31:$B$37)</f>
-        <v>1.0086996966079688E-2</v>
-      </c>
-      <c r="E31" s="1">
-        <f>SUM(C31:$C$37)</f>
-        <v>33919</v>
+        <v>4882</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="3">
-        <v>8</v>
-      </c>
-      <c r="B32" s="2">
-        <f t="shared" si="0"/>
-        <v>1.7923385334049436E-3</v>
-      </c>
-      <c r="C32" s="1">
-        <v>6027</v>
+      <c r="A32" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="1">
+        <v>848</v>
+      </c>
+      <c r="C32" s="2">
+        <f>B32/$E$2</f>
+        <v>6.2971076374707608E-3</v>
       </c>
       <c r="D32" s="2">
+        <f>SUM(C32:$C$37)</f>
+        <v>2.9688486243641628E-2</v>
+      </c>
+      <c r="E32" s="1">
         <f>SUM(B32:$B$37)</f>
-        <v>8.0029238879144576E-3</v>
-      </c>
-      <c r="E32" s="1">
-        <f>SUM(C32:$C$37)</f>
-        <v>26911</v>
+        <v>3998</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="3">
-        <v>0</v>
-      </c>
-      <c r="B33" s="2">
-        <f t="shared" si="0"/>
-        <v>1.695985839722647E-3</v>
-      </c>
-      <c r="C33" s="1">
-        <v>5703</v>
+      <c r="A33" s="8">
+        <v>8</v>
+      </c>
+      <c r="B33" s="1">
+        <v>797</v>
+      </c>
+      <c r="C33" s="2">
+        <f>B33/$E$2</f>
+        <v>5.9183900790851368E-3</v>
       </c>
       <c r="D33" s="2">
+        <f>SUM(C33:$C$37)</f>
+        <v>2.3391378606170868E-2</v>
+      </c>
+      <c r="E33" s="1">
         <f>SUM(B33:$B$37)</f>
-        <v>6.210585354509514E-3</v>
-      </c>
-      <c r="E33" s="1">
-        <f>SUM(C33:$C$37)</f>
-        <v>20884</v>
+        <v>3150</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="3">
+      <c r="A34" s="8">
         <v>9</v>
       </c>
-      <c r="B34" s="2">
-        <f t="shared" si="0"/>
-        <v>1.6347245591715571E-3</v>
-      </c>
-      <c r="C34" s="1">
-        <v>5497</v>
+      <c r="B34" s="1">
+        <v>759</v>
+      </c>
+      <c r="C34" s="2">
+        <f>B34/$E$2</f>
+        <v>5.6362083689154565E-3</v>
       </c>
       <c r="D34" s="2">
+        <f>SUM(C34:$C$37)</f>
+        <v>1.7472988527085731E-2</v>
+      </c>
+      <c r="E34" s="1">
         <f>SUM(B34:$B$37)</f>
-        <v>4.514599514786867E-3</v>
-      </c>
-      <c r="E34" s="1">
-        <f>SUM(C34:$C$37)</f>
-        <v>15181</v>
+        <v>2353</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B35" s="2">
-        <f t="shared" si="0"/>
-        <v>1.4726498120825088E-3</v>
-      </c>
-      <c r="C35" s="1">
-        <v>4952</v>
+      <c r="A35" s="8">
+        <v>0</v>
+      </c>
+      <c r="B35" s="1">
+        <v>741</v>
+      </c>
+      <c r="C35" s="2">
+        <f>B35/$E$2</f>
+        <v>5.5025433483087659E-3</v>
       </c>
       <c r="D35" s="2">
+        <f>SUM(C35:$C$37)</f>
+        <v>1.1836780158170274E-2</v>
+      </c>
+      <c r="E35" s="1">
         <f>SUM(B35:$B$37)</f>
-        <v>2.8798749556153101E-3</v>
-      </c>
-      <c r="E35" s="1">
-        <f>SUM(C35:$C$37)</f>
-        <v>9684</v>
+        <v>1594</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B36" s="2">
-        <f t="shared" si="0"/>
-        <v>9.2754336912062704E-4</v>
-      </c>
-      <c r="C36" s="1">
-        <v>3119</v>
+      <c r="A36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1">
+        <v>547</v>
+      </c>
+      <c r="C36" s="2">
+        <f>B36/$E$2</f>
+        <v>4.0619314595477666E-3</v>
       </c>
       <c r="D36" s="2">
+        <f>SUM(C36:$C$37)</f>
+        <v>6.3342368098615077E-3</v>
+      </c>
+      <c r="E36" s="1">
         <f>SUM(B36:$B$37)</f>
-        <v>1.4072251435328013E-3</v>
-      </c>
-      <c r="E36" s="1">
-        <f>SUM(C36:$C$37)</f>
-        <v>4732</v>
+        <v>853</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B37" s="2">
-        <f t="shared" si="0"/>
-        <v>4.7968177441217423E-4</v>
-      </c>
-      <c r="C37" s="1">
-        <v>1613</v>
+      <c r="B37" s="1">
+        <v>306</v>
+      </c>
+      <c r="C37" s="2">
+        <f>B37/$E$2</f>
+        <v>2.2723053503137416E-3</v>
       </c>
       <c r="D37" s="2">
+        <f>SUM(C37:$C$37)</f>
+        <v>2.2723053503137416E-3</v>
+      </c>
+      <c r="E37" s="1">
         <f>SUM(B37:$B$37)</f>
-        <v>4.7968177441217423E-4</v>
-      </c>
-      <c r="E37" s="1">
-        <f>SUM(C37:$C$37)</f>
-        <v>1613</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C37">
-    <sortCondition descending="1" ref="B2:B37"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E37">
+    <sortCondition descending="1" ref="B1:B37"/>
   </sortState>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>